<commit_message>
Quick push after trying to reproduce the today line error (RGB values non integer) before trying to solve within a user story (bug).
</commit_message>
<xml_diff>
--- a/source/tests/test_resources/input_files/config_files/KBT-VisualConfig.xlsx
+++ b/source/tests/test_resources/input_files/config_files/KBT-VisualConfig.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Development/PycharmProjects/ppt-plan-visual/source/tests/test_resources/input_files/config_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livestockinformation.sharepoint.com/sites/AddedValue/Shared Documents/General/Knowledge-Based Trading/Planning/DeliveryPlanning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93E8D886-A174-264A-A3AD-3E86E825AD86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="8_{5714A1EF-65DD-C543-9332-AB8A94813BAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D15686E6-06CC-424E-83D6-4E66A5F7C533}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="14140" xr2:uid="{974F07DA-9A00-0C4E-BD47-E61A1ACCDB18}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="3" xr2:uid="{974F07DA-9A00-0C4E-BD47-E61A1ACCDB18}"/>
   </bookViews>
   <sheets>
     <sheet name="PlotConfig" sheetId="1" r:id="rId1"/>
@@ -268,7 +268,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -305,6 +305,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -318,7 +324,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -333,6 +339,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -795,8 +802,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -912,10 +919,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{621F4AD7-AF79-4C43-ADFB-779A6ECDD917}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:R14"/>
+  <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView zoomScale="75" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView zoomScale="108" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1812,6 +1819,9 @@
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Font Colour Id]],ColourLookup[Id],ColourLookup[Blue],"xxx",0)</f>
         <v>xxx</v>
       </c>
+    </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F20" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1888,8 +1898,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B4:H18"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2343,16 +2353,16 @@
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{902C7751-B1B0-43AF-A6DD-8F0778B5A12C}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="dbd788b1-066a-4afa-a460-6ad1f8b5becc"/>
     <ds:schemaRef ds:uri="70221af8-9b81-45a2-828a-db5fddf7520d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
#179011884 When plotting today line, error because RGB values weren't integers
</commit_message>
<xml_diff>
--- a/source/tests/test_resources/input_files/config_files/KBT-VisualConfig.xlsx
+++ b/source/tests/test_resources/input_files/config_files/KBT-VisualConfig.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livestockinformation.sharepoint.com/sites/AddedValue/Shared Documents/General/Knowledge-Based Trading/Planning/DeliveryPlanning/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Development/PycharmProjects/ppt-plan-visual/source/tests/test_resources/input_files/config_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="8_{5714A1EF-65DD-C543-9332-AB8A94813BAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D15686E6-06CC-424E-83D6-4E66A5F7C533}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0BB4D78-A227-AF46-8C6A-FC37C5247D87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="3" xr2:uid="{974F07DA-9A00-0C4E-BD47-E61A1ACCDB18}"/>
+    <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="14140" activeTab="1" xr2:uid="{974F07DA-9A00-0C4E-BD47-E61A1ACCDB18}"/>
   </bookViews>
   <sheets>
     <sheet name="PlotConfig" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="70">
   <si>
     <t>Top</t>
   </si>
@@ -268,7 +268,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -305,12 +305,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -324,7 +318,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -339,7 +333,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -803,7 +796,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -919,10 +912,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{621F4AD7-AF79-4C43-ADFB-779A6ECDD917}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:R20"/>
+  <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView zoomScale="108" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="K2" zoomScale="171" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1782,7 +1775,9 @@
         <f>Table1[[#This Row],[Fill Colour Id]]</f>
         <v>DarkBlue</v>
       </c>
-      <c r="D14" s="7"/>
+      <c r="D14" s="7" t="s">
+        <v>38</v>
+      </c>
       <c r="E14" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Fill Colour Id]],ColourLookup[Id],ColourLookup[Red],"xxx",0)</f>
         <v>32</v>
@@ -1807,21 +1802,18 @@
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Line Colour Id]],ColourLookup[Id],ColourLookup[Blue],"xxx",0)</f>
         <v>100</v>
       </c>
-      <c r="O14" s="7" t="str">
+      <c r="O14" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Font Colour Id]],ColourLookup[Id],ColourLookup[Red],"xxx",0)</f>
-        <v>xxx</v>
-      </c>
-      <c r="P14" s="7" t="str">
+        <v>255</v>
+      </c>
+      <c r="P14" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Font Colour Id]],ColourLookup[Id],ColourLookup[Green],"xxx",0)</f>
-        <v>xxx</v>
-      </c>
-      <c r="Q14" s="7" t="str">
+        <v>255</v>
+      </c>
+      <c r="Q14" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Font Colour Id]],ColourLookup[Id],ColourLookup[Blue],"xxx",0)</f>
-        <v>xxx</v>
-      </c>
-    </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F20" s="10"/>
+        <v>255</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1898,8 +1890,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B4:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:E5"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2353,16 +2345,16 @@
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{902C7751-B1B0-43AF-A6DD-8F0778B5A12C}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="dbd788b1-066a-4afa-a460-6ad1f8b5becc"/>
     <ds:schemaRef ds:uri="70221af8-9b81-45a2-828a-db5fddf7520d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
#178922914 Remove dependency on Pandas
</commit_message>
<xml_diff>
--- a/source/tests/test_resources/input_files/config_files/KBT-VisualConfig.xlsx
+++ b/source/tests/test_resources/input_files/config_files/KBT-VisualConfig.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Development/PycharmProjects/ppt-plan-visual/source/tests/test_resources/input_files/config_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0BB4D78-A227-AF46-8C6A-FC37C5247D87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA0F775B-7BB8-5F4E-B126-19654784549D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="14140" activeTab="1" xr2:uid="{974F07DA-9A00-0C4E-BD47-E61A1ACCDB18}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="72">
   <si>
     <t>Top</t>
   </si>
@@ -247,6 +247,12 @@
   </si>
   <si>
     <t>diamond</t>
+  </si>
+  <si>
+    <t>Critical Path (Red)</t>
+  </si>
+  <si>
+    <t>Critical Path (Amber)</t>
   </si>
 </sst>
 </file>
@@ -426,8 +432,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3DFA5499-3D72-FD4D-98A8-9A364D6A060E}" name="Table1" displayName="Table1" ref="A1:R14" totalsRowShown="0" headerRowDxfId="11">
-  <autoFilter ref="A1:R14" xr:uid="{E2FE5099-2205-2446-9D79-AE0D6D124131}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3DFA5499-3D72-FD4D-98A8-9A364D6A060E}" name="Table1" displayName="Table1" ref="A1:R16" totalsRowShown="0" headerRowDxfId="11">
+  <autoFilter ref="A1:R16" xr:uid="{E2FE5099-2205-2446-9D79-AE0D6D124131}"/>
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{6F657443-D392-9749-8D22-77937F3594B4}" name="Format Name"/>
     <tableColumn id="18" xr3:uid="{A1AE67FA-1135-E249-8708-8700254B6C5E}" name="Fill Colour Id"/>
@@ -912,10 +918,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{621F4AD7-AF79-4C43-ADFB-779A6ECDD917}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:R14"/>
+  <dimension ref="A1:R16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K2" zoomScale="171" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="172" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1437,40 +1443,40 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
         <v>38</v>
       </c>
       <c r="E9">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Fill Colour Id]],ColourLookup[Id],ColourLookup[Red],"xxx",0)</f>
-        <v>0</v>
+        <v>255</v>
       </c>
       <c r="F9">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Fill Colour Id]],ColourLookup[Id],ColourLookup[Green],"xxx",0)</f>
-        <v>176</v>
+        <v>192</v>
       </c>
       <c r="G9">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Fill Colour Id]],ColourLookup[Id],ColourLookup[Blue],"xxx",0)</f>
-        <v>240</v>
+        <v>0</v>
       </c>
       <c r="H9">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Line Colour Id]],ColourLookup[Id],ColourLookup[Red],"xxx",0)</f>
-        <v>255</v>
+        <v>146</v>
       </c>
       <c r="I9">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Line Colour Id]],ColourLookup[Id],ColourLookup[Green],"xxx",0)</f>
-        <v>255</v>
+        <v>208</v>
       </c>
       <c r="J9">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Line Colour Id]],ColourLookup[Id],ColourLookup[Blue],"xxx",0)</f>
-        <v>255</v>
+        <v>80</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -1502,315 +1508,457 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[Fill Colour Id]],ColourLookup[Id],ColourLookup[Red],"xxx",0)</f>
+        <v>255</v>
+      </c>
+      <c r="F10">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[Fill Colour Id]],ColourLookup[Id],ColourLookup[Green],"xxx",0)</f>
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[Fill Colour Id]],ColourLookup[Id],ColourLookup[Blue],"xxx",0)</f>
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[Line Colour Id]],ColourLookup[Id],ColourLookup[Red],"xxx",0)</f>
+        <v>146</v>
+      </c>
+      <c r="I10">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[Line Colour Id]],ColourLookup[Id],ColourLookup[Green],"xxx",0)</f>
+        <v>208</v>
+      </c>
+      <c r="J10">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[Line Colour Id]],ColourLookup[Id],ColourLookup[Blue],"xxx",0)</f>
+        <v>80</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>7</v>
+      </c>
+      <c r="M10" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="N10" t="b">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[Font Colour Id]],ColourLookup[Id],ColourLookup[Red],"xxx",0)</f>
+        <v>255</v>
+      </c>
+      <c r="P10">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[Font Colour Id]],ColourLookup[Id],ColourLookup[Green],"xxx",0)</f>
+        <v>255</v>
+      </c>
+      <c r="Q10">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[Font Colour Id]],ColourLookup[Id],ColourLookup[Blue],"xxx",0)</f>
+        <v>255</v>
+      </c>
+      <c r="R10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[Fill Colour Id]],ColourLookup[Id],ColourLookup[Red],"xxx",0)</f>
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[Fill Colour Id]],ColourLookup[Id],ColourLookup[Green],"xxx",0)</f>
+        <v>176</v>
+      </c>
+      <c r="G11">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[Fill Colour Id]],ColourLookup[Id],ColourLookup[Blue],"xxx",0)</f>
+        <v>240</v>
+      </c>
+      <c r="H11">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[Line Colour Id]],ColourLookup[Id],ColourLookup[Red],"xxx",0)</f>
+        <v>255</v>
+      </c>
+      <c r="I11">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[Line Colour Id]],ColourLookup[Id],ColourLookup[Green],"xxx",0)</f>
+        <v>255</v>
+      </c>
+      <c r="J11">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[Line Colour Id]],ColourLookup[Id],ColourLookup[Blue],"xxx",0)</f>
+        <v>255</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>7</v>
+      </c>
+      <c r="M11" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="N11" t="b">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[Font Colour Id]],ColourLookup[Id],ColourLookup[Red],"xxx",0)</f>
+        <v>255</v>
+      </c>
+      <c r="P11">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[Font Colour Id]],ColourLookup[Id],ColourLookup[Green],"xxx",0)</f>
+        <v>255</v>
+      </c>
+      <c r="Q11">
+        <f>_xlfn.XLOOKUP(Table1[[#This Row],[Font Colour Id]],ColourLookup[Id],ColourLookup[Blue],"xxx",0)</f>
+        <v>255</v>
+      </c>
+      <c r="R11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>42</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="7" t="str">
+      <c r="C12" s="7" t="str">
         <f>Table1[[#This Row],[Fill Colour Id]]</f>
         <v>Light Grey</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D12" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E12" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Fill Colour Id]],ColourLookup[Id],ColourLookup[Red],"xxx",0)</f>
         <v>242</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F12" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Fill Colour Id]],ColourLookup[Id],ColourLookup[Green],"xxx",0)</f>
         <v>242</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G12" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Fill Colour Id]],ColourLookup[Id],ColourLookup[Blue],"xxx",0)</f>
         <v>242</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H12" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Line Colour Id]],ColourLookup[Id],ColourLookup[Red],"xxx",0)</f>
         <v>242</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I12" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Line Colour Id]],ColourLookup[Id],ColourLookup[Green],"xxx",0)</f>
         <v>242</v>
       </c>
-      <c r="J10" s="7">
+      <c r="J12" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Line Colour Id]],ColourLookup[Id],ColourLookup[Blue],"xxx",0)</f>
         <v>242</v>
       </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
         <v>14</v>
       </c>
-      <c r="M10" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="N10" t="b">
-        <v>0</v>
-      </c>
-      <c r="O10" s="7">
+      <c r="M12" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="N12" t="b">
+        <v>0</v>
+      </c>
+      <c r="O12" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Font Colour Id]],ColourLookup[Id],ColourLookup[Red],"xxx",0)</f>
         <v>166</v>
       </c>
-      <c r="P10" s="7">
+      <c r="P12" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Font Colour Id]],ColourLookup[Id],ColourLookup[Green],"xxx",0)</f>
         <v>166</v>
       </c>
-      <c r="Q10" s="7">
+      <c r="Q12" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Font Colour Id]],ColourLookup[Id],ColourLookup[Blue],"xxx",0)</f>
         <v>166</v>
       </c>
-      <c r="R10" t="s">
+      <c r="R12" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>45</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B13" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="7" t="str">
+      <c r="C13" s="7" t="str">
         <f>Table1[[#This Row],[Fill Colour Id]]</f>
         <v>White</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D13" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E13" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Fill Colour Id]],ColourLookup[Id],ColourLookup[Red],"xxx",0)</f>
         <v>255</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F13" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Fill Colour Id]],ColourLookup[Id],ColourLookup[Green],"xxx",0)</f>
         <v>255</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G13" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Fill Colour Id]],ColourLookup[Id],ColourLookup[Blue],"xxx",0)</f>
         <v>255</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H13" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Line Colour Id]],ColourLookup[Id],ColourLookup[Red],"xxx",0)</f>
         <v>255</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I13" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Line Colour Id]],ColourLookup[Id],ColourLookup[Green],"xxx",0)</f>
         <v>255</v>
       </c>
-      <c r="J11" s="7">
+      <c r="J13" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Line Colour Id]],ColourLookup[Id],ColourLookup[Blue],"xxx",0)</f>
         <v>255</v>
       </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
         <v>14</v>
       </c>
-      <c r="M11" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="N11" t="b">
-        <v>0</v>
-      </c>
-      <c r="O11" s="7">
+      <c r="M13" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="N13" t="b">
+        <v>0</v>
+      </c>
+      <c r="O13" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Font Colour Id]],ColourLookup[Id],ColourLookup[Red],"xxx",0)</f>
         <v>166</v>
       </c>
-      <c r="P11" s="7">
+      <c r="P13" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Font Colour Id]],ColourLookup[Id],ColourLookup[Green],"xxx",0)</f>
         <v>166</v>
       </c>
-      <c r="Q11" s="7">
+      <c r="Q13" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Font Colour Id]],ColourLookup[Id],ColourLookup[Blue],"xxx",0)</f>
         <v>166</v>
       </c>
-      <c r="R11" t="s">
+      <c r="R13" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>52</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B14" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="7" t="str">
+      <c r="C14" s="7" t="str">
         <f>Table1[[#This Row],[Fill Colour Id]]</f>
         <v>Light Green</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D14" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E14" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Fill Colour Id]],ColourLookup[Id],ColourLookup[Red],"xxx",0)</f>
         <v>241</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F14" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Fill Colour Id]],ColourLookup[Id],ColourLookup[Green],"xxx",0)</f>
         <v>246</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G14" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Fill Colour Id]],ColourLookup[Id],ColourLookup[Blue],"xxx",0)</f>
         <v>213</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H14" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Line Colour Id]],ColourLookup[Id],ColourLookup[Red],"xxx",0)</f>
         <v>241</v>
       </c>
-      <c r="I12" s="7">
+      <c r="I14" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Line Colour Id]],ColourLookup[Id],ColourLookup[Green],"xxx",0)</f>
         <v>246</v>
       </c>
-      <c r="J12" s="7">
+      <c r="J14" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Line Colour Id]],ColourLookup[Id],ColourLookup[Blue],"xxx",0)</f>
         <v>213</v>
       </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
         <v>14</v>
       </c>
-      <c r="M12" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="N12" t="b">
-        <v>0</v>
-      </c>
-      <c r="O12" s="7">
+      <c r="M14" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="N14" t="b">
+        <v>0</v>
+      </c>
+      <c r="O14" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Font Colour Id]],ColourLookup[Id],ColourLookup[Red],"xxx",0)</f>
         <v>32</v>
       </c>
-      <c r="P12" s="7">
+      <c r="P14" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Font Colour Id]],ColourLookup[Id],ColourLookup[Green],"xxx",0)</f>
         <v>56</v>
       </c>
-      <c r="Q12" s="7">
+      <c r="Q14" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Font Colour Id]],ColourLookup[Id],ColourLookup[Blue],"xxx",0)</f>
         <v>100</v>
       </c>
-      <c r="R12" t="s">
+      <c r="R14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>53</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B15" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="7" t="str">
+      <c r="C15" s="7" t="str">
         <f>Table1[[#This Row],[Fill Colour Id]]</f>
         <v>Very Light Green</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D15" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E15" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Fill Colour Id]],ColourLookup[Id],ColourLookup[Red],"xxx",0)</f>
         <v>214</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F15" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Fill Colour Id]],ColourLookup[Id],ColourLookup[Green],"xxx",0)</f>
         <v>227</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G15" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Fill Colour Id]],ColourLookup[Id],ColourLookup[Blue],"xxx",0)</f>
         <v>130</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H15" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Line Colour Id]],ColourLookup[Id],ColourLookup[Red],"xxx",0)</f>
         <v>214</v>
       </c>
-      <c r="I13" s="7">
+      <c r="I15" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Line Colour Id]],ColourLookup[Id],ColourLookup[Green],"xxx",0)</f>
         <v>227</v>
       </c>
-      <c r="J13" s="7">
+      <c r="J15" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Line Colour Id]],ColourLookup[Id],ColourLookup[Blue],"xxx",0)</f>
         <v>130</v>
       </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
         <v>14</v>
       </c>
-      <c r="M13" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="N13" t="b">
-        <v>0</v>
-      </c>
-      <c r="O13" s="7">
+      <c r="M15" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="N15" t="b">
+        <v>0</v>
+      </c>
+      <c r="O15" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Font Colour Id]],ColourLookup[Id],ColourLookup[Red],"xxx",0)</f>
         <v>32</v>
       </c>
-      <c r="P13" s="7">
+      <c r="P15" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Font Colour Id]],ColourLookup[Id],ColourLookup[Green],"xxx",0)</f>
         <v>56</v>
       </c>
-      <c r="Q13" s="7">
+      <c r="Q15" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Font Colour Id]],ColourLookup[Id],ColourLookup[Blue],"xxx",0)</f>
         <v>100</v>
       </c>
-      <c r="R13" t="s">
+      <c r="R15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>65</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B16" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="7" t="str">
+      <c r="C16" s="7" t="str">
         <f>Table1[[#This Row],[Fill Colour Id]]</f>
         <v>DarkBlue</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D16" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E16" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Fill Colour Id]],ColourLookup[Id],ColourLookup[Red],"xxx",0)</f>
         <v>32</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F16" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Fill Colour Id]],ColourLookup[Id],ColourLookup[Green],"xxx",0)</f>
         <v>56</v>
       </c>
-      <c r="G14" s="7">
+      <c r="G16" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Fill Colour Id]],ColourLookup[Id],ColourLookup[Blue],"xxx",0)</f>
         <v>100</v>
       </c>
-      <c r="H14" s="7">
+      <c r="H16" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Line Colour Id]],ColourLookup[Id],ColourLookup[Red],"xxx",0)</f>
         <v>32</v>
       </c>
-      <c r="I14" s="7">
+      <c r="I16" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Line Colour Id]],ColourLookup[Id],ColourLookup[Green],"xxx",0)</f>
         <v>56</v>
       </c>
-      <c r="J14" s="7">
+      <c r="J16" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Line Colour Id]],ColourLookup[Id],ColourLookup[Blue],"xxx",0)</f>
         <v>100</v>
       </c>
-      <c r="O14" s="7">
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>14</v>
+      </c>
+      <c r="M16" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="N16" t="b">
+        <v>0</v>
+      </c>
+      <c r="O16" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Font Colour Id]],ColourLookup[Id],ColourLookup[Red],"xxx",0)</f>
         <v>255</v>
       </c>
-      <c r="P14" s="7">
+      <c r="P16" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Font Colour Id]],ColourLookup[Id],ColourLookup[Green],"xxx",0)</f>
         <v>255</v>
       </c>
-      <c r="Q14" s="7">
+      <c r="Q16" s="7">
         <f>_xlfn.XLOOKUP(Table1[[#This Row],[Font Colour Id]],ColourLookup[Id],ColourLookup[Blue],"xxx",0)</f>
         <v>255</v>
       </c>

</xml_diff>